<commit_message>
Stable - Players are not lost (with comments and system-prints)
</commit_message>
<xml_diff>
--- a/PerformanceComparisonsStrategies.xlsx
+++ b/PerformanceComparisonsStrategies.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sascha\eclipse-workspace\MATSim\tcDietlikon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1555FE91-04AC-4E8C-AA6B-CE33F3B4515C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5706BEE2-150B-4044-9158-4F8F63218C30}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{02913CC5-923C-4EE8-83BB-E17D286254B7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{02913CC5-923C-4EE8-83BB-E17D286254B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="67">
   <si>
     <t>Player Set 1</t>
   </si>
@@ -165,14 +167,88 @@
   </si>
   <si>
     <t>{0=0, 1=11, 2=10, 3=0, 4=152, 5=0, 6=0, 7=0, 8=44}</t>
+  </si>
+  <si>
+    <t>{0=0, 1=16, 2=22, 3=0, 4=136, 5=0, 6=0, 7=0, 8=40, 9=0}</t>
+  </si>
+  <si>
+    <t>break; push; pushLevel=3</t>
+  </si>
+  <si>
+    <t>{0=0, 1=17, 2=20, 3=0, 4=136, 5=0, 6=0, 7=0, 8=40, 9=0}</t>
+  </si>
+  <si>
+    <t>BENCHMARK</t>
+  </si>
+  <si>
+    <t>Shift</t>
+  </si>
+  <si>
+    <t>Unused</t>
+  </si>
+  <si>
+    <t>Initial</t>
+  </si>
+  <si>
+    <t>0=0, 1=16, 2=26, 3=6, 4=172</t>
+  </si>
+  <si>
+    <t>0=0, 1=12, 2=25, 3=0, 4=183</t>
+  </si>
+  <si>
+    <t>0=206, 1=9, 2=4, 3=1, 4=0</t>
+  </si>
+  <si>
+    <t>0=0, 1=15, 2=26, 3=6, 4=168</t>
+  </si>
+  <si>
+    <t>0=0, 1=15, 2=28, 3=3, 4=168</t>
+  </si>
+  <si>
+    <t>0=0, 1=15, 2=26, 3=3, 4=172</t>
+  </si>
+  <si>
+    <t>w/ G4 (&lt;-1)</t>
+  </si>
+  <si>
+    <t>w/o G4 (&lt;-1)</t>
+  </si>
+  <si>
+    <t>w/o G4 (&lt;-0)</t>
+  </si>
+  <si>
+    <t>0=0, 1=15, 2=26, 3=3, 4=176</t>
+  </si>
+  <si>
+    <t>New dataset I</t>
+  </si>
+  <si>
+    <t>0=0, 1=19, 2=10, 3=12, 4=144, 5=0, 6=6, 7=0, 8=32, 9=0</t>
+  </si>
+  <si>
+    <t>0=0, 1=8, 2=7, 3=0, 4=169, 5=0, 6=0, 7=0, 8=39</t>
+  </si>
+  <si>
+    <t>0=187, 1=16, 2=13, 3=6, 4=0, 5=0, 6=0, 7=1</t>
+  </si>
+  <si>
+    <t>0=0, 1=17, 2=10, 3=9, 4=148, 5=0, 6=6, 7=0, 8=32, 9=0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -200,8 +276,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -516,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA124D4-F2C5-47F4-A174-CFB2AFF13CCC}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -719,6 +796,17 @@
         <v>32</v>
       </c>
     </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>40</v>
@@ -736,6 +824,212 @@
       </c>
       <c r="D29" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D261B55-67EB-4C94-B555-2658B1110625}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="26.88671875" customWidth="1"/>
+    <col min="4" max="4" width="29.77734375" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{176CE647-B533-4A23-89EE-822A5EEA0279}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="50" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
G5 post optimization stable
</commit_message>
<xml_diff>
--- a/PerformanceComparisonsStrategies.xlsx
+++ b/PerformanceComparisonsStrategies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sascha\eclipse-workspace\MATSim\tcDietlikon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA01E0D9-E720-4881-97D9-5D1E3A9F8AD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409DAF8F-A8B1-4251-AEF9-25AF80735D69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{02913CC5-923C-4EE8-83BB-E17D286254B7}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="88">
   <si>
     <t>Player Set 1</t>
   </si>
@@ -254,6 +254,48 @@
   </si>
   <si>
     <t>{0=0, 1=16, 2=12, 3=9, 4=176, 5=0, 6=6, 7=0, 8=8, 9=0}</t>
+  </si>
+  <si>
+    <t>without new placement strategy</t>
+  </si>
+  <si>
+    <t>0=0, 1=48, 2=12, 3=27, 4=124, 5=5, 6=0, 7=0, 8=0, 9=0</t>
+  </si>
+  <si>
+    <t>0=0, 1=50, 2=0, 3=13, 4=161, 5=0, 6=0, 7=0, 8=11</t>
+  </si>
+  <si>
+    <t>0=0, 1=44, 2=16, 3=27, 4=124, 5=5, 6=0, 7=0, 8=0, 9=0</t>
+  </si>
+  <si>
+    <t>0=0, 1=43, 2=14, 3=18, 4=136, 5=5, 6=0, 7=0, 8=0, 9=0</t>
+  </si>
+  <si>
+    <t>nUnsatisfied</t>
+  </si>
+  <si>
+    <t>{0=0, 1=42, 2=4, 3=24, 4=128, 5=5, 6=0, 7=0, 8=0, 9=0</t>
+  </si>
+  <si>
+    <t>0=0, 1=59, 2=14, 3=57, 4=68, 5=5, 6=0, 7=0, 8=0, 9=0</t>
+  </si>
+  <si>
+    <t>0=0, 1=43, 2=14, 3=18, 4=136, 5=5</t>
+  </si>
+  <si>
+    <t>0=0, 1=48, 2=12, 3=27, 4=124, 5=5</t>
+  </si>
+  <si>
+    <t>0=0, 1=40, 2=6, 3=24, 4=132, 5=5, 6=0, 7=0, 8=0, 9=0</t>
+  </si>
+  <si>
+    <t>{0=0, 1=60, 2=26, 3=36, 4=80, 5=5, 6=0, 7=0, 8=0, 9=0}</t>
+  </si>
+  <si>
+    <t>0=0, 1=40, 2=8, 3=15, 4=136, 5=5</t>
+  </si>
+  <si>
+    <t>0=0, 1=40, 2=6, 3=21, 4=132, 5=5</t>
   </si>
 </sst>
 </file>
@@ -969,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{176CE647-B533-4A23-89EE-822A5EEA0279}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1071,6 +1113,83 @@
         <v>49</v>
       </c>
     </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" t="s">
+        <v>83</v>
+      </c>
+      <c r="F23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>